<commit_message>
Minor changes to wording
</commit_message>
<xml_diff>
--- a/Backend/Report.xlsx
+++ b/Backend/Report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>EEID</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>Jake Doe</t>
   </si>
   <si>
     <t>Joe Doe</t>
@@ -93,7 +96,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -140,7 +143,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>42.34</v>
+        <v>54.34</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -178,23 +181,34 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="0" t="n">
-        <v>9988</v>
+        <v>5555</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>99.88</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="0" t="n">
-        <v>9999</v>
+        <v>9988</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="n">
+        <v>99.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="0" t="n">
+        <v>9999</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>39.44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made small changes to front end
</commit_message>
<xml_diff>
--- a/Backend/Report.xlsx
+++ b/Backend/Report.xlsx
@@ -22,10 +22,10 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Jess Doe</t>
+    <t>John Doe</t>
   </si>
   <si>
-    <t>June Doe</t>
+    <t>Jane Doe</t>
   </si>
 </sst>
 </file>
@@ -94,18 +94,18 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="0" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>4</v>

</xml_diff>